<commit_message>
Individulas in Objects Aggiornamento dati
</commit_message>
<xml_diff>
--- a/Dati/50volumi.xlsx
+++ b/Dati/50volumi.xlsx
@@ -1,46 +1,128 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MODUNIVAR\Shiny\Dati\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RSTUDIOAPPLICATIVI\Modunivar-master\Dati\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B1113E-07A6-41B2-867E-9386369CD757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B665975F-E076-40FA-BD5C-C133D10AB646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
-    <sheet name="Foglio2" sheetId="2" r:id="rId2"/>
+    <sheet name="dataset" sheetId="1" r:id="rId1"/>
+    <sheet name="Dati per lezione" sheetId="2" r:id="rId2"/>
     <sheet name="Foglio3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="17">
   <si>
     <t>Volume</t>
+  </si>
+  <si>
+    <t>Trial#</t>
+  </si>
+  <si>
+    <t>Volume (mL)</t>
+  </si>
+  <si>
+    <t>minimum</t>
+  </si>
+  <si>
+    <t>maximum</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>standard dev.</t>
+  </si>
+  <si>
+    <t>mL</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>IQR (Q3-Q1)</t>
+  </si>
+  <si>
+    <t>RSD%</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>max-min</t>
+  </si>
+  <si>
+    <t>Fat table</t>
+  </si>
+  <si>
+    <t>Slim table</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Lucida Sans Unicode"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Lucida Sans Unicode"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -51,7 +133,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -59,13 +141,100 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -83,10 +252,90 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>123826</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="CasellaDiTesto 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86360182-1A3D-BF5F-CC70-288E9CBD256A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3581400" y="2466976"/>
+          <a:ext cx="2286000" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100"/>
+            <a:t>Random generated data for</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100" baseline="0"/>
+            <a:t> exercise</a:t>
+          </a:r>
+          <a:endParaRPr lang="it-IT" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -124,9 +373,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -159,26 +408,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -211,26 +443,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -406,264 +621,266 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>9.9660978998690837</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>9.9876565513659727</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>9.9840829857021447</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>9.9762499125609168</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>9.985478953658486</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>9.9845911631382762</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>9.9790652770571171</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>9.966347261488437</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9.9880948186728631</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9.9883172628870227</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9.9756648982838954</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>9.9883709703681518</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>9.98153272708808</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>9.9828889874152367</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>9.973997890901984</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>9.9791621491567923</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>9.9786628211041091</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>9.9945338847283267</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>9.985033976099686</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>9.9797675170157447</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>9.98161006687954</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>9.9766584357530803</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>9.9849568655008909</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>9.9760833404252764</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>9.9815138059603044</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>9.9858255502659006</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>9.9718180394666263</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>9.9834067145457368</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>9.9841787818695877</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>9.9873038747864769</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>9.9742074748610605</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>9.9752335704215795</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>9.9849726352295249</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>9.9773061851556406</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>9.9815481975929572</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>9.9773565184114261</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>9.9807356522979092</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>9.9932558045657345</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>9.9897677723311347</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>9.9731393351794679</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>9.9837531456251156</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>9.9889932921178399</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>9.9892381844802287</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>9.9853341102607658</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>9.9789043265082285</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>9.9788009797157713</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>9.979934452039771</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>9.9746345117273734</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>9.9766907519188237</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>9.9747410353848238</v>
       </c>
@@ -675,13 +892,873 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M52"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="13"/>
+    <col min="13" max="13" width="13.5703125" style="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5">
+        <v>9.9110084815584116</v>
+      </c>
+      <c r="C3" s="4">
+        <v>11</v>
+      </c>
+      <c r="D3" s="5">
+        <v>10.007252461455238</v>
+      </c>
+      <c r="E3" s="4">
+        <v>21</v>
+      </c>
+      <c r="F3" s="5">
+        <v>9.9912990433131483</v>
+      </c>
+      <c r="G3" s="4">
+        <v>31</v>
+      </c>
+      <c r="H3" s="5">
+        <v>9.9563299667898093</v>
+      </c>
+      <c r="I3" s="4">
+        <v>41</v>
+      </c>
+      <c r="J3" s="5">
+        <v>9.9975310431182436</v>
+      </c>
+      <c r="L3" s="13">
+        <v>1</v>
+      </c>
+      <c r="M3" s="14">
+        <v>9.9110084815584116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7">
+        <v>9.9935676925815926</v>
+      </c>
+      <c r="C4" s="6">
+        <v>12</v>
+      </c>
+      <c r="D4" s="7">
+        <v>9.9688985582907037</v>
+      </c>
+      <c r="E4" s="6">
+        <v>22</v>
+      </c>
+      <c r="F4" s="7">
+        <v>9.9121217030733817</v>
+      </c>
+      <c r="G4" s="6">
+        <v>32</v>
+      </c>
+      <c r="H4" s="7">
+        <v>10.009209011932427</v>
+      </c>
+      <c r="I4" s="6">
+        <v>42</v>
+      </c>
+      <c r="J4" s="7">
+        <v>10.010202066459925</v>
+      </c>
+      <c r="L4" s="13">
+        <v>2</v>
+      </c>
+      <c r="M4" s="14">
+        <v>9.9935676925815926</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>3</v>
+      </c>
+      <c r="B5" s="7">
+        <v>9.9537182959102495</v>
+      </c>
+      <c r="C5" s="6">
+        <v>13</v>
+      </c>
+      <c r="D5" s="7">
+        <v>10.01044183200068</v>
+      </c>
+      <c r="E5" s="6">
+        <v>23</v>
+      </c>
+      <c r="F5" s="7">
+        <v>9.9799139602146454</v>
+      </c>
+      <c r="G5" s="6">
+        <v>33</v>
+      </c>
+      <c r="H5" s="7">
+        <v>9.9859686938180232</v>
+      </c>
+      <c r="I5" s="6">
+        <v>43</v>
+      </c>
+      <c r="J5" s="7">
+        <v>9.9462762986695736</v>
+      </c>
+      <c r="L5" s="13">
+        <v>3</v>
+      </c>
+      <c r="M5" s="14">
+        <v>9.9537182959102495</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7">
+        <v>9.9693310230213967</v>
+      </c>
+      <c r="C6" s="6">
+        <v>14</v>
+      </c>
+      <c r="D6" s="7">
+        <v>9.9671018799290607</v>
+      </c>
+      <c r="E6" s="6">
+        <v>24</v>
+      </c>
+      <c r="F6" s="7">
+        <v>10.037954842537175</v>
+      </c>
+      <c r="G6" s="6">
+        <v>34</v>
+      </c>
+      <c r="H6" s="7">
+        <v>9.9955445361593149</v>
+      </c>
+      <c r="I6" s="6">
+        <v>44</v>
+      </c>
+      <c r="J6" s="7">
+        <v>9.9720335581060056</v>
+      </c>
+      <c r="L6" s="13">
+        <v>4</v>
+      </c>
+      <c r="M6" s="14">
+        <v>9.9693310230213967</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>5</v>
+      </c>
+      <c r="B7" s="7">
+        <v>9.9802592271408059</v>
+      </c>
+      <c r="C7" s="6">
+        <v>15</v>
+      </c>
+      <c r="D7" s="7">
+        <v>9.9581537310405395</v>
+      </c>
+      <c r="E7" s="6">
+        <v>25</v>
+      </c>
+      <c r="F7" s="7">
+        <v>9.9952002924146939</v>
+      </c>
+      <c r="G7" s="6">
+        <v>35</v>
+      </c>
+      <c r="H7" s="7">
+        <v>9.9555863411842722</v>
+      </c>
+      <c r="I7" s="6">
+        <v>45</v>
+      </c>
+      <c r="J7" s="7">
+        <v>9.9798294908942182</v>
+      </c>
+      <c r="L7" s="13">
+        <v>5</v>
+      </c>
+      <c r="M7" s="14">
+        <v>9.9802592271408059</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>6</v>
+      </c>
+      <c r="B8" s="7">
+        <v>9.9990783494013442</v>
+      </c>
+      <c r="C8" s="6">
+        <v>16</v>
+      </c>
+      <c r="D8" s="7">
+        <v>9.936544819047441</v>
+      </c>
+      <c r="E8" s="6">
+        <v>26</v>
+      </c>
+      <c r="F8" s="7">
+        <v>9.9882799756506131</v>
+      </c>
+      <c r="G8" s="6">
+        <v>36</v>
+      </c>
+      <c r="H8" s="7">
+        <v>9.9917267047749476</v>
+      </c>
+      <c r="I8" s="6">
+        <v>46</v>
+      </c>
+      <c r="J8" s="7">
+        <v>10.005678012439631</v>
+      </c>
+      <c r="L8" s="13">
+        <v>6</v>
+      </c>
+      <c r="M8" s="14">
+        <v>9.9990783494013442</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>7</v>
+      </c>
+      <c r="B9" s="7">
+        <v>9.9472119413440225</v>
+      </c>
+      <c r="C9" s="6">
+        <v>17</v>
+      </c>
+      <c r="D9" s="7">
+        <v>9.9517927250963396</v>
+      </c>
+      <c r="E9" s="6">
+        <v>27</v>
+      </c>
+      <c r="F9" s="7">
+        <v>9.995270692988953</v>
+      </c>
+      <c r="G9" s="6">
+        <v>37</v>
+      </c>
+      <c r="H9" s="7">
+        <v>9.9610454694448265</v>
+      </c>
+      <c r="I9" s="6">
+        <v>47</v>
+      </c>
+      <c r="J9" s="7">
+        <v>9.9799830249685613</v>
+      </c>
+      <c r="L9" s="13">
+        <v>7</v>
+      </c>
+      <c r="M9" s="14">
+        <v>9.9472119413440225</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>8</v>
+      </c>
+      <c r="B10" s="7">
+        <v>9.9612701714795833</v>
+      </c>
+      <c r="C10" s="6">
+        <v>18</v>
+      </c>
+      <c r="D10" s="7">
+        <v>9.9763555906156682</v>
+      </c>
+      <c r="E10" s="6">
+        <v>28</v>
+      </c>
+      <c r="F10" s="7">
+        <v>10.032249127525603</v>
+      </c>
+      <c r="G10" s="6">
+        <v>38</v>
+      </c>
+      <c r="H10" s="7">
+        <v>10.016677555049711</v>
+      </c>
+      <c r="I10" s="6">
+        <v>48</v>
+      </c>
+      <c r="J10" s="7">
+        <v>9.9424434606226271</v>
+      </c>
+      <c r="L10" s="13">
+        <v>8</v>
+      </c>
+      <c r="M10" s="14">
+        <v>9.9612701714795833</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>9</v>
+      </c>
+      <c r="B11" s="7">
+        <v>9.9898265429692685</v>
+      </c>
+      <c r="C11" s="6">
+        <v>19</v>
+      </c>
+      <c r="D11" s="7">
+        <v>10.013220054097502</v>
+      </c>
+      <c r="E11" s="6">
+        <v>29</v>
+      </c>
+      <c r="F11" s="7">
+        <v>10.014313323572452</v>
+      </c>
+      <c r="G11" s="6">
+        <v>39</v>
+      </c>
+      <c r="H11" s="7">
+        <v>9.9968844208069925</v>
+      </c>
+      <c r="I11" s="6">
+        <v>49</v>
+      </c>
+      <c r="J11" s="7">
+        <v>9.9681800290545937</v>
+      </c>
+      <c r="L11" s="13">
+        <v>9</v>
+      </c>
+      <c r="M11" s="14">
+        <v>9.9898265429692685</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>10</v>
+      </c>
+      <c r="B12" s="9">
+        <v>9.9677186594454099</v>
+      </c>
+      <c r="C12" s="8">
+        <v>20</v>
+      </c>
+      <c r="D12" s="9">
+        <v>9.9727788037489802</v>
+      </c>
+      <c r="E12" s="8">
+        <v>30</v>
+      </c>
+      <c r="F12" s="9">
+        <v>9.9491183559257763</v>
+      </c>
+      <c r="G12" s="8">
+        <v>40</v>
+      </c>
+      <c r="H12" s="9">
+        <v>9.9582979996376082</v>
+      </c>
+      <c r="I12" s="8">
+        <v>50</v>
+      </c>
+      <c r="J12" s="9">
+        <v>9.9495939079679658</v>
+      </c>
+      <c r="L12" s="13">
+        <v>10</v>
+      </c>
+      <c r="M12" s="14">
+        <v>9.9677186594454099</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L13" s="13">
+        <v>11</v>
+      </c>
+      <c r="M13" s="14">
+        <v>10.007252461455238</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="2">
+        <f>MIN(B3:B12,D3:D12,F3:F12,H3:H12,J3:J12)</f>
+        <v>9.9110084815584116</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L14" s="13">
+        <v>12</v>
+      </c>
+      <c r="M14" s="14">
+        <v>9.9688985582907037</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="2">
+        <f>+MAX(B3:B12,D3:D12,F3:F12,H3:H12,J3:J12)</f>
+        <v>10.037954842537175</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L15" s="13">
+        <v>13</v>
+      </c>
+      <c r="M15" s="14">
+        <v>10.01044183200068</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="2">
+        <f>C15-C14</f>
+        <v>0.12694636097876355</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L16" s="13">
+        <v>14</v>
+      </c>
+      <c r="M16" s="14">
+        <v>9.9671018799290607</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="2">
+        <f>+AVERAGE(B3:B12,D3:D12,F3:F12,H3:H12,J3:J12)</f>
+        <v>9.9782054749857867</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L17" s="13">
+        <v>15</v>
+      </c>
+      <c r="M17" s="14">
+        <v>9.9581537310405395</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="2">
+        <f>+MEDIAN(B3:B12,D3:D12,F3:F12,H3:H12,J3:J12)</f>
+        <v>9.9798717255544318</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L18" s="13">
+        <v>16</v>
+      </c>
+      <c r="M18" s="14">
+        <v>9.936544819047441</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="2">
+        <f>+_xlfn.STDEV.S(B3:B12,D3:D12,F3:F12,H3:H12,J3:J12)</f>
+        <v>2.7789652442345041E-2</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L19" s="13">
+        <v>17</v>
+      </c>
+      <c r="M19" s="14">
+        <v>9.9517927250963396</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="12">
+        <f>C19/C17*100</f>
+        <v>0.27850350959408987</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L20" s="13">
+        <v>18</v>
+      </c>
+      <c r="M20" s="14">
+        <v>9.9763555906156682</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="2">
+        <f>_xlfn.PERCENTILE.EXC(M3:M52,0.25)</f>
+        <v>9.9576977899778569</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L21" s="13">
+        <v>19</v>
+      </c>
+      <c r="M21" s="14">
+        <v>10.013220054097502</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="2">
+        <f>_xlfn.PERCENTILE.EXC(M:M, 0.75)</f>
+        <v>9.9970460763848052</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L22" s="13">
+        <v>20</v>
+      </c>
+      <c r="M22" s="14">
+        <v>9.9727788037489802</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="2">
+        <f>C22-C21</f>
+        <v>3.9348286406948318E-2</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L23" s="13">
+        <v>21</v>
+      </c>
+      <c r="M23" s="14">
+        <v>9.9912990433131483</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L24" s="13">
+        <v>22</v>
+      </c>
+      <c r="M24" s="14">
+        <v>9.9121217030733817</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L25" s="13">
+        <v>23</v>
+      </c>
+      <c r="M25" s="14">
+        <v>9.9799139602146454</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L26" s="13">
+        <v>24</v>
+      </c>
+      <c r="M26" s="14">
+        <v>10.037954842537175</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L27" s="13">
+        <v>25</v>
+      </c>
+      <c r="M27" s="14">
+        <v>9.9952002924146939</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L28" s="13">
+        <v>26</v>
+      </c>
+      <c r="M28" s="14">
+        <v>9.9882799756506131</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L29" s="13">
+        <v>27</v>
+      </c>
+      <c r="M29" s="14">
+        <v>9.995270692988953</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L30" s="13">
+        <v>28</v>
+      </c>
+      <c r="M30" s="14">
+        <v>10.032249127525603</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L31" s="13">
+        <v>29</v>
+      </c>
+      <c r="M31" s="14">
+        <v>10.014313323572452</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L32" s="13">
+        <v>30</v>
+      </c>
+      <c r="M32" s="14">
+        <v>9.9491183559257763</v>
+      </c>
+    </row>
+    <row r="33" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L33" s="13">
+        <v>31</v>
+      </c>
+      <c r="M33" s="14">
+        <v>9.9563299667898093</v>
+      </c>
+    </row>
+    <row r="34" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L34" s="13">
+        <v>32</v>
+      </c>
+      <c r="M34" s="14">
+        <v>10.009209011932427</v>
+      </c>
+    </row>
+    <row r="35" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L35" s="13">
+        <v>33</v>
+      </c>
+      <c r="M35" s="14">
+        <v>9.9859686938180232</v>
+      </c>
+    </row>
+    <row r="36" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L36" s="13">
+        <v>34</v>
+      </c>
+      <c r="M36" s="14">
+        <v>9.9955445361593149</v>
+      </c>
+    </row>
+    <row r="37" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L37" s="13">
+        <v>35</v>
+      </c>
+      <c r="M37" s="14">
+        <v>9.9555863411842722</v>
+      </c>
+    </row>
+    <row r="38" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L38" s="13">
+        <v>36</v>
+      </c>
+      <c r="M38" s="14">
+        <v>9.9917267047749476</v>
+      </c>
+    </row>
+    <row r="39" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L39" s="13">
+        <v>37</v>
+      </c>
+      <c r="M39" s="14">
+        <v>9.9610454694448265</v>
+      </c>
+    </row>
+    <row r="40" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L40" s="13">
+        <v>38</v>
+      </c>
+      <c r="M40" s="14">
+        <v>10.016677555049711</v>
+      </c>
+    </row>
+    <row r="41" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L41" s="13">
+        <v>39</v>
+      </c>
+      <c r="M41" s="14">
+        <v>9.9968844208069925</v>
+      </c>
+    </row>
+    <row r="42" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L42" s="13">
+        <v>40</v>
+      </c>
+      <c r="M42" s="14">
+        <v>9.9582979996376082</v>
+      </c>
+    </row>
+    <row r="43" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L43" s="13">
+        <v>41</v>
+      </c>
+      <c r="M43" s="14">
+        <v>9.9975310431182436</v>
+      </c>
+    </row>
+    <row r="44" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L44" s="13">
+        <v>42</v>
+      </c>
+      <c r="M44" s="14">
+        <v>10.010202066459925</v>
+      </c>
+    </row>
+    <row r="45" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L45" s="13">
+        <v>43</v>
+      </c>
+      <c r="M45" s="14">
+        <v>9.9462762986695736</v>
+      </c>
+    </row>
+    <row r="46" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L46" s="13">
+        <v>44</v>
+      </c>
+      <c r="M46" s="14">
+        <v>9.9720335581060056</v>
+      </c>
+    </row>
+    <row r="47" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L47" s="13">
+        <v>45</v>
+      </c>
+      <c r="M47" s="14">
+        <v>9.9798294908942182</v>
+      </c>
+    </row>
+    <row r="48" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L48" s="13">
+        <v>46</v>
+      </c>
+      <c r="M48" s="14">
+        <v>10.005678012439631</v>
+      </c>
+    </row>
+    <row r="49" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L49" s="13">
+        <v>47</v>
+      </c>
+      <c r="M49" s="14">
+        <v>9.9799830249685613</v>
+      </c>
+    </row>
+    <row r="50" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L50" s="13">
+        <v>48</v>
+      </c>
+      <c r="M50" s="14">
+        <v>9.9424434606226271</v>
+      </c>
+    </row>
+    <row r="51" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L51" s="13">
+        <v>49</v>
+      </c>
+      <c r="M51" s="14">
+        <v>9.9681800290545937</v>
+      </c>
+    </row>
+    <row r="52" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L52" s="13">
+        <v>50</v>
+      </c>
+      <c r="M52" s="14">
+        <v>9.9495939079679658</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -691,7 +1768,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>